<commit_message>
Added manual REX hours
</commit_message>
<xml_diff>
--- a/assets/projet_A.xlsx
+++ b/assets/projet_A.xlsx
@@ -885,37 +885,37 @@
         <v>0</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>55.2228875582169</v>
+        <v>87.15000000000001</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>9.481037924151698</v>
+        <v>14.9625</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>85.26280771789754</v>
+        <v>134.5575</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J2" s="4" t="n">
-        <v>3.992015968063872</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="K2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="L2" s="4" t="n">
-        <v>51.23087159015303</v>
+        <v>80.85000000000001</v>
       </c>
       <c r="M2" s="4" t="n">
-        <v>111.5036593479707</v>
+        <v>175.9695</v>
       </c>
       <c r="N2" s="4" t="n">
-        <v>59.48103792415171</v>
+        <v>93.87</v>
       </c>
       <c r="O2" s="4" t="n">
-        <v>421.8296739853626</v>
+        <v>665.7105</v>
       </c>
       <c r="P2" s="4" t="n">
-        <v>2.661343978709248</v>
+        <v>4.2</v>
       </c>
       <c r="Q2" s="4" t="n">
         <v>0</v>
@@ -930,22 +930,22 @@
         <v>0</v>
       </c>
       <c r="U2" s="4" t="n">
-        <v>66.60013306719894</v>
+        <v>105.105</v>
       </c>
       <c r="V2" s="4" t="n">
-        <v>8.183632734530939</v>
+        <v>12.915</v>
       </c>
       <c r="W2" s="4" t="n">
-        <v>9.514304723885564</v>
+        <v>15.015</v>
       </c>
       <c r="X2" s="4" t="n">
-        <v>16.36726546906188</v>
+        <v>25.83</v>
       </c>
       <c r="Y2" s="4" t="n">
-        <v>26.81304058549567</v>
+        <v>42.315</v>
       </c>
       <c r="Z2" s="4" t="n">
-        <v>18.62940785096474</v>
+        <v>29.4</v>
       </c>
       <c r="AA2" s="4" t="n">
         <v>0</v>
@@ -957,13 +957,13 @@
         <v>0</v>
       </c>
       <c r="AD2" s="4" t="n">
-        <v>2.328675981370592</v>
+        <v>3.675</v>
       </c>
       <c r="AE2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="AF2" s="4" t="n">
-        <v>3.659347970725217</v>
+        <v>5.775</v>
       </c>
       <c r="AG2" s="4" t="n">
         <v>0</v>
@@ -984,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="AM2" s="4" t="n">
-        <v>17.29873586161012</v>
+        <v>27.3</v>
       </c>
       <c r="AN2" s="4" t="n">
         <v>0</v>
@@ -1002,22 +1002,22 @@
         <v>0</v>
       </c>
       <c r="AS2" s="4" t="n">
-        <v>15.30272787757818</v>
+        <v>24.15</v>
       </c>
       <c r="AT2" s="4" t="n">
-        <v>1.330671989354624</v>
+        <v>2.1</v>
       </c>
       <c r="AU2" s="4" t="n">
-        <v>2.661343978709248</v>
+        <v>4.2</v>
       </c>
       <c r="AV2" s="4" t="n">
-        <v>1.330671989354624</v>
+        <v>2.1</v>
       </c>
       <c r="AW2" s="4" t="n">
-        <v>3.992015968063872</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="AX2" s="4" t="n">
-        <v>5.322687957418497</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>